<commit_message>
update details about zircon
</commit_message>
<xml_diff>
--- a/DataFileSamples/Others/Cluster.xlsx
+++ b/DataFileSamples/Others/Cluster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/Others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{21D6BD4C-81BE-F44E-9A4A-A86DA046C731}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{18DB4115-5D40-0A4B-92C5-7109277BA4DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20120" yWindow="6700" windowWidth="17440" windowHeight="16940" xr2:uid="{412D788D-48D5-5042-9445-1F4F49743A84}"/>
+    <workbookView xWindow="5920" yWindow="3440" windowWidth="17440" windowHeight="16940" xr2:uid="{412D788D-48D5-5042-9445-1F4F49743A84}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Author</t>
   </si>
@@ -441,7 +441,47 @@
     <t>*</t>
   </si>
   <si>
-    <t>green</t>
+    <t>Group1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -875,67 +915,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273537D0-6113-6F4C-BD6E-9D8467FE2467}">
-  <dimension ref="A1:AS9"/>
+  <dimension ref="A1:AL9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="J1" sqref="J1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:38" ht="18">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="C1" s="5" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
@@ -958,420 +983,237 @@
       <c r="AJ1" s="5"/>
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:38">
       <c r="A2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>56</v>
+        <v>69</v>
+      </c>
+      <c r="B2" s="6">
+        <v>50</v>
       </c>
       <c r="C2" s="6">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E2" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
       </c>
       <c r="H2" s="6">
-        <v>1</v>
+        <v>1024</v>
       </c>
       <c r="I2" s="6">
         <v>1024</v>
       </c>
-      <c r="J2" s="6">
-        <v>1024</v>
-      </c>
-      <c r="K2" s="6">
-        <v>1024</v>
-      </c>
-      <c r="L2" s="6">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="M2" s="6">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="N2" s="6">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="O2" s="6">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="P2" s="6">
-        <f>O2*3</f>
-        <v>26.400000000000002</v>
-      </c>
     </row>
-    <row r="3" spans="1:45">
+    <row r="3" spans="1:38">
       <c r="A3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>56</v>
+        <v>69</v>
+      </c>
+      <c r="B3" s="6">
+        <v>50</v>
       </c>
       <c r="C3" s="6">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D3" s="6">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="6">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
       </c>
       <c r="H3" s="6">
-        <v>1</v>
+        <v>715</v>
       </c>
       <c r="I3" s="6">
         <v>715</v>
       </c>
-      <c r="J3" s="6">
-        <v>715</v>
-      </c>
-      <c r="K3" s="6">
-        <v>715</v>
-      </c>
-      <c r="L3" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="M3" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="N3" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="O3" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="P3" s="6">
-        <f t="shared" ref="P3:P9" si="0">O3*3</f>
-        <v>47.7</v>
-      </c>
     </row>
-    <row r="4" spans="1:45">
-      <c r="A4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>56</v>
+    <row r="4" spans="1:38">
+      <c r="A4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="6">
+        <v>50</v>
       </c>
       <c r="C4" s="6">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E4" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="6">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G4" s="6">
         <v>1</v>
       </c>
       <c r="H4" s="6">
-        <v>1</v>
+        <v>870</v>
       </c>
       <c r="I4" s="6">
         <v>870</v>
       </c>
-      <c r="J4" s="6">
-        <v>870</v>
-      </c>
-      <c r="K4" s="6">
-        <v>870</v>
-      </c>
-      <c r="L4" s="6">
-        <v>15.2</v>
-      </c>
-      <c r="M4" s="6">
-        <v>15.2</v>
-      </c>
-      <c r="N4" s="6">
-        <v>15.2</v>
-      </c>
-      <c r="O4" s="6">
-        <v>15.2</v>
-      </c>
-      <c r="P4" s="6">
-        <f t="shared" si="0"/>
-        <v>45.599999999999994</v>
-      </c>
     </row>
-    <row r="5" spans="1:45">
-      <c r="A5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>64</v>
+    <row r="5" spans="1:38">
+      <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="6">
+        <v>30</v>
       </c>
       <c r="C5" s="6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F5" s="6">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G5" s="6">
         <v>3</v>
       </c>
       <c r="H5" s="6">
-        <v>3</v>
+        <v>1025</v>
       </c>
       <c r="I5" s="6">
         <v>1025</v>
       </c>
-      <c r="J5" s="6">
-        <v>1025</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1025</v>
-      </c>
-      <c r="L5" s="6">
-        <v>23.8</v>
-      </c>
-      <c r="M5" s="6">
-        <v>23.8</v>
-      </c>
-      <c r="N5" s="6">
-        <v>23.8</v>
-      </c>
-      <c r="O5" s="6">
-        <v>23.8</v>
-      </c>
-      <c r="P5" s="6">
-        <f t="shared" si="0"/>
-        <v>71.400000000000006</v>
-      </c>
     </row>
-    <row r="6" spans="1:45">
-      <c r="A6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>64</v>
+    <row r="6" spans="1:38">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="6">
+        <v>30</v>
       </c>
       <c r="C6" s="6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D6" s="6">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E6" s="6">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F6" s="6">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6">
         <v>3</v>
       </c>
       <c r="H6" s="6">
-        <v>3</v>
+        <v>902</v>
       </c>
       <c r="I6" s="6">
         <v>902</v>
       </c>
-      <c r="J6" s="6">
-        <v>902</v>
-      </c>
-      <c r="K6" s="6">
-        <v>902</v>
-      </c>
-      <c r="L6" s="6">
-        <v>21.4</v>
-      </c>
-      <c r="M6" s="6">
-        <v>21.4</v>
-      </c>
-      <c r="N6" s="6">
-        <v>21.4</v>
-      </c>
-      <c r="O6" s="6">
-        <v>21.4</v>
-      </c>
-      <c r="P6" s="6">
-        <f t="shared" si="0"/>
-        <v>64.199999999999989</v>
-      </c>
     </row>
-    <row r="7" spans="1:45">
-      <c r="A7" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>69</v>
+    <row r="7" spans="1:38">
+      <c r="A7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="6">
+        <v>40</v>
       </c>
       <c r="C7" s="6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F7" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="6">
         <v>3</v>
       </c>
       <c r="H7" s="6">
-        <v>3</v>
+        <v>941</v>
       </c>
       <c r="I7" s="6">
         <v>941</v>
       </c>
-      <c r="J7" s="6">
-        <v>941</v>
-      </c>
-      <c r="K7" s="6">
-        <v>941</v>
-      </c>
-      <c r="L7" s="6">
-        <v>13.6</v>
-      </c>
-      <c r="M7" s="6">
-        <v>13.6</v>
-      </c>
-      <c r="N7" s="6">
-        <v>13.6</v>
-      </c>
-      <c r="O7" s="6">
-        <v>13.6</v>
-      </c>
-      <c r="P7" s="6">
-        <f t="shared" si="0"/>
-        <v>40.799999999999997</v>
-      </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:38">
       <c r="A8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="B8" s="6">
+        <v>40</v>
       </c>
       <c r="C8" s="6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E8" s="6">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F8" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="6">
         <v>3</v>
       </c>
       <c r="H8" s="6">
-        <v>3</v>
+        <v>995</v>
       </c>
       <c r="I8" s="6">
         <v>995</v>
       </c>
-      <c r="J8" s="6">
-        <v>995</v>
-      </c>
-      <c r="K8" s="6">
-        <v>995</v>
-      </c>
-      <c r="L8" s="6">
-        <v>17.8</v>
-      </c>
-      <c r="M8" s="6">
-        <v>17.8</v>
-      </c>
-      <c r="N8" s="6">
-        <v>17.8</v>
-      </c>
-      <c r="O8" s="6">
-        <v>17.8</v>
-      </c>
-      <c r="P8" s="6">
-        <f t="shared" si="0"/>
-        <v>53.400000000000006</v>
-      </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:38">
       <c r="A9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="B9" s="6">
+        <v>40</v>
       </c>
       <c r="C9" s="6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D9" s="6">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E9" s="6">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F9" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="6">
         <v>3</v>
       </c>
       <c r="H9" s="6">
-        <v>3</v>
+        <v>700</v>
       </c>
       <c r="I9" s="6">
         <v>700</v>
-      </c>
-      <c r="J9" s="6">
-        <v>700</v>
-      </c>
-      <c r="K9" s="6">
-        <v>700</v>
-      </c>
-      <c r="L9" s="6">
-        <v>9.6</v>
-      </c>
-      <c r="M9" s="6">
-        <v>9.6</v>
-      </c>
-      <c r="N9" s="6">
-        <v>9.6</v>
-      </c>
-      <c r="O9" s="6">
-        <v>9.6</v>
-      </c>
-      <c r="P9" s="6">
-        <f t="shared" si="0"/>
-        <v>28.799999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>